<commit_message>
Test 4 runs successfully! I also added Home Page and Login Page some verification and PageFactory Web elements. -Muharrem
</commit_message>
<xml_diff>
--- a/src/main/resources/automation-exercise-data.xlsx
+++ b/src/main/resources/automation-exercise-data.xlsx
@@ -70,13 +70,13 @@
     <t>Lee</t>
   </si>
   <si>
-    <t>TechCentureKevinLee123@gmail.com</t>
+    <t>kevinlee123@gmail.com</t>
   </si>
   <si>
     <t>kevinlee123456@gmail.com</t>
   </si>
   <si>
-    <t>NoPassword1</t>
+    <t>No Password</t>
   </si>
   <si>
     <t>KevinLeeTechCenturegmail.com</t>
@@ -165,10 +165,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -189,6 +189,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -202,6 +210,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -211,113 +250,74 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -338,19 +338,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -362,157 +410,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -523,6 +523,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -550,32 +565,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -595,6 +589,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -602,15 +611,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -628,139 +628,139 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1108,7 +1108,7 @@
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>

</xml_diff>

<commit_message>
added test case 2-3.
</commit_message>
<xml_diff>
--- a/src/main/resources/automation-exercise-data.xlsx
+++ b/src/main/resources/automation-exercise-data.xlsx
@@ -165,10 +165,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -197,6 +197,75 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -210,9 +279,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -226,16 +301,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -248,80 +322,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -338,6 +338,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -350,169 +356,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -545,7 +545,16 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -561,30 +570,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -619,7 +604,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -628,139 +628,139 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -773,11 +773,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="48" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1107,8 +1110,8 @@
   <sheetPr/>
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1188,7 +1191,7 @@
       <c r="D2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -1232,10 +1235,10 @@
       <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>29</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1279,10 +1282,10 @@
       <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>33</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -1326,10 +1329,10 @@
       <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>37</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -1373,10 +1376,10 @@
       <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -1420,10 +1423,10 @@
       <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>45</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -1458,18 +1461,21 @@
       </c>
     </row>
     <row r="8" spans="4:5">
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="4:5">
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="4:5">
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="kevinlee123@gmail.com"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Test Case 5 is done by Muharrem. It runs successfully
</commit_message>
<xml_diff>
--- a/src/main/resources/automation-exercise-data.xlsx
+++ b/src/main/resources/automation-exercise-data.xlsx
@@ -165,10 +165,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -182,90 +182,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -280,14 +196,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -301,20 +232,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -322,6 +239,89 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -338,175 +338,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -523,6 +523,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -537,6 +561,47 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -558,212 +623,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1110,8 +1110,8 @@
   <sheetPr/>
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>

</xml_diff>

<commit_message>
created Contact Page for Test 6. It works!
</commit_message>
<xml_diff>
--- a/src/main/resources/automation-exercise-data.xlsx
+++ b/src/main/resources/automation-exercise-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15620"/>
+    <workbookView windowHeight="15640"/>
   </bookViews>
   <sheets>
     <sheet name="CustomerAccountInformation" sheetId="1" r:id="rId1"/>
@@ -165,10 +165,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -182,6 +182,126 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -195,129 +315,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -338,181 +338,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -523,30 +523,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -606,6 +582,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -623,147 +614,156 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">

</xml_diff>

<commit_message>
Created first test case register user
</commit_message>
<xml_diff>
--- a/src/main/resources/automation-exercise-data.xlsx
+++ b/src/main/resources/automation-exercise-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15620"/>
+    <workbookView windowHeight="15520"/>
   </bookViews>
   <sheets>
     <sheet name="CustomerAccountInformation" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="54">
   <si>
     <t>Run</t>
   </si>
@@ -61,6 +61,15 @@
     <t>Zip</t>
   </si>
   <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>DateOfBirth</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
     <t>y</t>
   </si>
   <si>
@@ -97,6 +106,12 @@
     <t>McLean</t>
   </si>
   <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
     <t>n</t>
   </si>
   <si>
@@ -110,6 +125,9 @@
   </si>
   <si>
     <t>Manhattan</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
   <si>
     <t>Oleysa</t>
@@ -166,9 +184,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -182,6 +200,111 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -195,15 +318,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -212,112 +336,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -332,19 +350,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -356,19 +482,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -380,139 +524,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -535,6 +553,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -546,6 +573,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -565,17 +616,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -594,176 +641,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -773,7 +791,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -788,6 +806,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="48" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1108,10 +1129,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1119,7 +1140,7 @@
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="14.1875" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="34.75" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.125" style="1" customWidth="1"/>
     <col min="5" max="5" width="24.8125" style="1" customWidth="1"/>
     <col min="6" max="6" width="17.1875" style="1" customWidth="1"/>
     <col min="7" max="7" width="16.5625" style="1" customWidth="1"/>
@@ -1129,9 +1150,10 @@
     <col min="11" max="11" width="13.1875" style="1" customWidth="1"/>
     <col min="12" max="12" width="14.4375" style="1" customWidth="1"/>
     <col min="13" max="15" width="9" style="1"/>
+    <col min="17" max="17" width="9.625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1177,287 +1199,350 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:18">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="O2" s="1">
         <v>25401</v>
       </c>
+      <c r="P2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>34778</v>
+      </c>
+      <c r="R2" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:18">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="O3" s="1">
         <v>25401</v>
       </c>
+      <c r="P3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>34778</v>
+      </c>
+      <c r="R3" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:18">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="O4" s="1">
         <v>25401</v>
       </c>
+      <c r="P4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>34778</v>
+      </c>
+      <c r="R4" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:18">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="O5" s="1">
         <v>25401</v>
       </c>
+      <c r="P5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>34778</v>
+      </c>
+      <c r="R5" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:18">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="O6" s="1">
         <v>25401</v>
       </c>
+      <c r="P6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>34778</v>
+      </c>
+      <c r="R6" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:18">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="O7" s="1">
         <v>25401</v>
+      </c>
+      <c r="P7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>34778</v>
+      </c>
+      <c r="R7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="4:5">

</xml_diff>